<commit_message>
updated examples and databases
</commit_message>
<xml_diff>
--- a/_MUT_USERBIN/CLN.xlsx
+++ b/_MUT_USERBIN/CLN.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Grdbldr\MUT_Examples\_MUT_USERBIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{772F5209-7A12-4C6A-9D12-9B5850A242DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA8F117-E899-4391-872A-A5F45242C68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A2A2007-294D-4F5E-BAF0-6B6DE97E3EBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{3A2A2007-294D-4F5E-BAF0-6B6DE97E3EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="CLN" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -59,9 +59,6 @@
     <t>Flow Treatment</t>
   </si>
   <si>
-    <t>Default CLN, a 10 cm well</t>
-  </si>
-  <si>
     <t>METERS</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>Unconfined/Mannings</t>
   </si>
   <si>
-    <t>CLN_for_SWF</t>
-  </si>
-  <si>
     <t>Confined Well</t>
   </si>
   <si>
@@ -159,6 +153,12 @@
   </si>
   <si>
     <t>Angled</t>
+  </si>
+  <si>
+    <t>2D Hillslope 100 m length</t>
+  </si>
+  <si>
+    <t>Default CLN a 10 cm well</t>
   </si>
 </sst>
 </file>
@@ -1007,8 +1007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2466777-6214-46BD-AE31-7E3BE048D9A7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1064,7 @@
         <v>3</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1072,16 +1072,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F2">
         <v>0.1</v>
@@ -1093,16 +1093,16 @@
         <v>1</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>5.4800000000000001E-2</v>
       </c>
       <c r="J2" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" t="s">
         <v>13</v>
-      </c>
-      <c r="L2" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1111,22 +1111,22 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="G3">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1135,13 +1135,13 @@
         <v>1</v>
       </c>
       <c r="J3" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="K3" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" t="s">
         <v>13</v>
-      </c>
-      <c r="L3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1150,37 +1150,37 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4" t="s">
         <v>21</v>
       </c>
-      <c r="F4">
-        <v>0.1</v>
-      </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4">
-        <v>5.4800000000000001E-2</v>
-      </c>
-      <c r="J4" t="s">
-        <v>22</v>
-      </c>
       <c r="K4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" t="s">
         <v>13</v>
-      </c>
-      <c r="L4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1189,16 +1189,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>17</v>
       </c>
       <c r="F5">
         <v>0.1</v>
@@ -1213,13 +1213,13 @@
         <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="K5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" t="s">
         <v>13</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1228,16 +1228,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
       </c>
       <c r="F6">
         <v>0.1</v>
@@ -1252,13 +1252,13 @@
         <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="L6" t="s">
         <v>13</v>
-      </c>
-      <c r="L6" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:13" customFormat="1" x14ac:dyDescent="0.25">
@@ -1267,16 +1267,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>17</v>
       </c>
       <c r="F7">
         <v>0.1</v>
@@ -1291,17 +1291,17 @@
         <v>1</v>
       </c>
       <c r="J7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="K7" t="s">
+        <v>12</v>
+      </c>
+      <c r="L7" t="s">
         <v>13</v>
       </c>
-      <c r="L7" t="s">
-        <v>14</v>
-      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="ICR7cNMXCB5fXve0PJb8qC4dS9kibbLVax9SlKEIrdR2tCuCbayuMFYkr2gjNdGgyqYt2sCWvgxGHbTQVPKHYw==" saltValue="zpOVhHxKKFutw7ck8HhMig==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="qCrYivdpSEJvqf5gopE82lAlXzAfPiGdn8a35lDDXC9tO18vDPL/KYRVgorRq/xfKQY2VjVszSS4X0vgwODmYg==" saltValue="tnfpcpW1jLGjAz0VADeH2w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
@@ -1352,21 +1352,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B06D2A-BC87-438F-9C8C-B5601E7E72C6}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>31</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1383,93 +1383,93 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="C2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes when finalizing manual
</commit_message>
<xml_diff>
--- a/_MUT_USERBIN/CLN.xlsx
+++ b/_MUT_USERBIN/CLN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repos\Grdbldr\MUT_Examples\_MUT_USERBIN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA8F117-E899-4391-872A-A5F45242C68B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2B83F5-CD36-4407-8BEF-76EC29DDE6F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{3A2A2007-294D-4F5E-BAF0-6B6DE97E3EBF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{3A2A2007-294D-4F5E-BAF0-6B6DE97E3EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="CLN" sheetId="1" r:id="rId1"/>
@@ -1007,9 +1007,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2466777-6214-46BD-AE31-7E3BE048D9A7}">
   <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1352,8 +1350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95B06D2A-BC87-438F-9C8C-B5601E7E72C6}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="24" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>